<commit_message>
manual search complete, next uncheck
</commit_message>
<xml_diff>
--- a/data/Repair_matrix DF.xlsx
+++ b/data/Repair_matrix DF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\twintern\Auto Purchase\AutoPurchase\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77109753-9EE4-49CB-862B-275C24D10BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A53A5BF-9691-4784-82E9-831CBF944095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="368" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -794,10 +794,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>Arm B</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>DM LIKA UPGRADE</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
@@ -807,6 +803,9 @@
   </si>
   <si>
     <t>V-700144</t>
+  </si>
+  <si>
+    <t>Arm B</t>
   </si>
 </sst>
 </file>
@@ -3085,8 +3084,8 @@
   </sheetPr>
   <dimension ref="A1:AE110"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -3539,7 +3538,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="271" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D21" s="68">
         <f>'Calc.'!H42</f>
@@ -3565,7 +3564,7 @@
         <v>198</v>
       </c>
       <c r="C22" s="271" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D22" s="68">
         <f>'Calc.'!H47</f>
@@ -3716,7 +3715,7 @@
         <v>142</v>
       </c>
       <c r="C29" s="271" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D29" s="68">
         <f>'Calc.'!I61</f>
@@ -3898,7 +3897,7 @@
         <v>151</v>
       </c>
       <c r="C36" s="273" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D36" s="68">
         <f>'Calc.'!I68</f>
@@ -4142,7 +4141,7 @@
         <v>202</v>
       </c>
       <c r="C46" s="272" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D46" s="142">
         <f>'Calc.'!G108</f>
@@ -4228,7 +4227,7 @@
         <v>12</v>
       </c>
       <c r="C50" s="271" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D50" s="68">
         <f>'Calc.'!I89</f>

</xml_diff>